<commit_message>
Add HPing to NS excel file
</commit_message>
<xml_diff>
--- a/excel-files/naming-service/SI-PS-PU-TI.xlsx
+++ b/excel-files/naming-service/SI-PS-PU-TI.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3493" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3501" uniqueCount="178">
   <si>
     <t>Super Section</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>InjDpK</t>
+  </si>
+  <si>
+    <t>HPing</t>
   </si>
   <si>
     <t>InjNLK</t>
@@ -664,10 +667,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G852"/>
+  <dimension ref="A1:G854"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A806" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E836" activeCellId="0" sqref="E836"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A829" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E852" activeCellId="0" sqref="E852"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12807,7 +12810,7 @@
         <v>7</v>
       </c>
       <c r="C849" s="3" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="D849" s="3" t="s">
         <v>172</v>
@@ -12821,13 +12824,13 @@
         <v>7</v>
       </c>
       <c r="C850" s="3" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="D850" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E850" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="E850" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="851" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12838,10 +12841,10 @@
         <v>171</v>
       </c>
       <c r="D851" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E851" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="852" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12849,13 +12852,41 @@
         <v>7</v>
       </c>
       <c r="C852" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D852" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E852" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="853" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B853" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C853" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D853" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E853" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="854" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B854" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C854" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D852" s="3" t="s">
+      <c r="D854" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E854" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="E852" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>